<commit_message>
[yerim] Ap 와 Actor data 분리, monsterskillbase 생성
</commit_message>
<xml_diff>
--- a/GameData/Excel/actor_rsc.xlsx
+++ b/GameData/Excel/actor_rsc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\Go.D.Taekwon\GameData\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yerim\portfolio_Game\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF7D2EE-6B8F-4B5B-82E0-E1A7D0819F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5284F78F-FA42-491D-9ABC-E59876C6D3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5928" yWindow="6924" windowWidth="34560" windowHeight="18792" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
   <sheets>
     <sheet name="actor_rsc" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>int</t>
   </si>
@@ -72,6 +72,12 @@
   <si>
     <t>액터 리소스 프리팹</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ActorPlayer</t>
+  </si>
+  <si>
+    <t>ActorEnemy</t>
   </si>
 </sst>
 </file>
@@ -508,17 +514,17 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" style="3" customWidth="1"/>
     <col min="3" max="3" width="25" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.796875" style="3"/>
+    <col min="4" max="16384" width="8.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -529,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -540,7 +546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" s="5" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -549,90 +555,94 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1000001</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2000001</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>

</xml_diff>